<commit_message>
Add Database Reset in Options and working form in imports
</commit_message>
<xml_diff>
--- a/Win32/Release/700 Produit Supirate.xlsx
+++ b/Win32/Release/700 Produit Supirate.xlsx
@@ -4339,7 +4339,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="\P00000"/>
     <numFmt numFmtId="165" formatCode="\P0000"/>
-    <numFmt numFmtId="170" formatCode="00"/>
+    <numFmt numFmtId="166" formatCode="00"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -4844,15 +4844,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5178,7 +5178,7 @@
   <dimension ref="A1:R715"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>